<commit_message>
Better clarity between Edwards and Govindaraju data
</commit_message>
<xml_diff>
--- a/fuelData/gcData/posf10325_init.xlsx
+++ b/fuelData/gcData/posf10325_init.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abinswan/Documents/GroupContributionMethod/Init_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/dmontgo2_nrel_gov/Documents/Projects/SAF-VTO/GCM/ismomeric-study/python/FuelLib/fuelData/gcData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE43A7AB-E91B-404D-9B73-33829119F801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{CE43A7AB-E91B-404D-9B73-33829119F801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93CCD911-F552-044E-A1D7-A8BA358F2714}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23460" windowHeight="14560" tabRatio="234" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41100" yWindow="1880" windowWidth="23460" windowHeight="14560" tabRatio="234" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Toluene</t>
   </si>
@@ -221,6 +234,12 @@
   </si>
   <si>
     <t>C12-Tricycloparaffin</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -275,9 +294,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -315,7 +334,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -421,7 +440,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -563,7 +582,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -571,9 +590,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B68"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -581,6 +602,14 @@
     <col min="2" max="1025" width="11.5"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
@@ -1125,4 +1154,10 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{95965d95-ecc0-4720-b759-1f33c42ed7da}" enabled="1" method="Standard" siteId="{a0f29d7e-28cd-4f54-8442-7885aee7c080}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>